<commit_message>
Organized Folder | Added Full Flow
</commit_message>
<xml_diff>
--- a/Data Files/Senior_Companion_Data_CaringConn.xlsx
+++ b/Data Files/Senior_Companion_Data_CaringConn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dilip Sunar\git\common-repo\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8B263C-59AE-40A1-8362-656FF4DA7E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3BE4AA-1120-44E5-9525-ECF4638B881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{A4DF82C4-8118-4B38-8D30-1F820878FD09}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{A4DF82C4-8118-4B38-8D30-1F820878FD09}"/>
   </bookViews>
   <sheets>
     <sheet name="Senior_Regression" sheetId="1" r:id="rId1"/>
@@ -1279,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED4CC9D-0592-479C-B19E-F0DCD2311CF0}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1623,7 +1623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D38EEC9-5651-4FB5-BE61-3FCB28F1E2B5}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>